<commit_message>
updated manufacture 2024 folder
</commit_message>
<xml_diff>
--- a/design_files/worklib/pc065b_fibv2_toplevel/physical/manufacture 2024/bill of materials.xlsx
+++ b/design_files/worklib/pc065b_fibv2_toplevel/physical/manufacture 2024/bill of materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ppfs6.physics.ox.ac.uk\CEG\Central Electronics\Projects\Hastingsp\DUNE\uob-hep-pc065\design_files\worklib\pc065b_fibv2_toplevel\physical\manufacture 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F24BD3-F456-428A-BC77-80DFD1D61A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5A3108-3432-4ECF-BF23-A4A22CD6B1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="1650" windowWidth="28800" windowHeight="15345" xr2:uid="{F89D0B4F-2DBE-4679-BEF7-16FC5DEE2B0A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15390" windowHeight="7785" xr2:uid="{F89D0B4F-2DBE-4679-BEF7-16FC5DEE2B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>MLZ2012DR10DT</t>
   </si>
   <si>
-    <t>TYCO 2007132</t>
-  </si>
-  <si>
     <t>TYCO 1888247-1</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>0402DC-4N7XGRW</t>
+  </si>
+  <si>
+    <t>TYCO 2007132-1</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB52B35-0EB8-4FBE-95A0-CA35294B5EBC}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -1086,7 +1086,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
@@ -1122,7 +1122,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1170,7 +1170,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1184,7 +1184,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1198,7 +1198,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1246,7 +1246,7 @@
         <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1292,7 +1292,7 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1306,7 +1306,7 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>

</xml_diff>